<commit_message>
Planning Test Plan Updates
</commit_message>
<xml_diff>
--- a/Technical/Testing/TestPlan.xlsx
+++ b/Technical/Testing/TestPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FlyNet\Technical\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\FlyNet\Technical\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -728,6 +728,19 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,19 +801,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,14 +1512,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="H1" s="24"/>
+      <c r="J1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="24"/>
       <c r="M1" t="s">
         <v>72</v>
       </c>
@@ -1577,19 +1577,19 @@
         <f>B9</f>
         <v>Initial Camera Test</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="26">
         <f>AVERAGE(AVERAGE(F3:F7),A5,AVERAGE(F3:F7),AVERAGE(F3:F7))</f>
         <v>0</v>
       </c>
-      <c r="J3" s="36" t="str">
+      <c r="J3" s="41" t="str">
         <f>B5</f>
         <v>Guidance Subsystem</v>
       </c>
-      <c r="L3" s="39">
+      <c r="L3" s="20">
         <f>AVERAGE(AVERAGE(I3,I9,I15,I21,I26),A3,AVERAGE(I3,I9,I15,I21,I26),AVERAGE(I3,I9,I15,I21,I26))</f>
         <v>0</v>
       </c>
-      <c r="M3" s="40" t="str">
+      <c r="M3" s="21" t="str">
         <f>B3</f>
         <v>End of Semester Test Demo</v>
       </c>
@@ -1615,10 +1615,10 @@
         <f>B10</f>
         <v>Target Imaging</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="37"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="41"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="42"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -1642,10 +1642,10 @@
         <v>Obstacle Perceived</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="37"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="41"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="42"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1669,10 +1669,10 @@
         <v>Obstacle Map</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="37"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="41"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="42"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -1698,10 +1698,10 @@
       <c r="H7" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="41"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="43"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
@@ -1716,8 +1716,8 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="39"/>
-      <c r="M8" s="41"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1740,16 +1740,16 @@
         <f>B11</f>
         <v>Human Target ID</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="27">
         <f>AVERAGE(AVERAGE(F9:F13),A4,AVERAGE(F9:F13),AVERAGE(F9:F13))</f>
         <v>0</v>
       </c>
-      <c r="J9" s="23" t="str">
+      <c r="J9" s="28" t="str">
         <f>B4</f>
         <v>Tracking/ID Subsystem</v>
       </c>
-      <c r="L9" s="39"/>
-      <c r="M9" s="41"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -1775,10 +1775,10 @@
         <f t="shared" si="0"/>
         <v>Target Estimation</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="24"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="41"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="29"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -1804,10 +1804,10 @@
         <f t="shared" si="0"/>
         <v>Multiple targets</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="24"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="41"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="29"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -1833,10 +1833,10 @@
         <f t="shared" si="0"/>
         <v>Target Estimate Update</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="24"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="41"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="29"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
@@ -1862,10 +1862,10 @@
         <f>B25</f>
         <v>Target Accuracy and Range</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="25"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="41"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="30"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
@@ -1884,8 +1884,8 @@
         <v>70</v>
       </c>
       <c r="F14"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="41"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="22"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
@@ -1911,16 +1911,16 @@
         <f t="shared" si="1"/>
         <v>Collision Correction Planning</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="34">
         <f>AVERAGE(AVERAGE(F15:F19),A6,AVERAGE(F15:F19),AVERAGE(F15:F19))</f>
         <v>0</v>
       </c>
-      <c r="J15" s="26" t="str">
+      <c r="J15" s="31" t="str">
         <f>B6</f>
         <v>Planning Subsystem</v>
       </c>
-      <c r="L15" s="39"/>
-      <c r="M15" s="41"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
@@ -1946,10 +1946,10 @@
         <f t="shared" si="1"/>
         <v>Trajectory Test Planning</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="27"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="41"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="32"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
@@ -1972,10 +1972,10 @@
         <f t="shared" si="1"/>
         <v>Obstacle Avoidance Planning</v>
       </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="27"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="41"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="32"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
@@ -1997,10 +1997,10 @@
       <c r="G18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="27"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="41"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="32"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="22"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
@@ -2025,10 +2025,10 @@
       <c r="G19" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="28"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="41"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="33"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="22"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
@@ -2043,8 +2043,8 @@
       <c r="D20" t="s">
         <v>47</v>
       </c>
-      <c r="L20" s="39"/>
-      <c r="M20" s="41"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="22"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
@@ -2060,23 +2060,23 @@
         <v>52</v>
       </c>
       <c r="F21" s="12">
-        <f>A27</f>
+        <f t="shared" ref="F21:G23" si="2">A27</f>
         <v>0</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f>B27</f>
+        <f t="shared" si="2"/>
         <v>Collision Correction Controls</v>
       </c>
-      <c r="I21" s="30">
+      <c r="I21" s="35">
         <f>AVERAGE(AVERAGE(F21:F24),A7,AVERAGE(F21:F24),AVERAGE(F21:F24))</f>
         <v>0</v>
       </c>
-      <c r="J21" s="31" t="str">
+      <c r="J21" s="36" t="str">
         <f>B7</f>
         <v>Controls Subsystem</v>
       </c>
-      <c r="L21" s="39"/>
-      <c r="M21" s="41"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
@@ -2092,17 +2092,17 @@
         <v>55</v>
       </c>
       <c r="F22" s="12">
-        <f>A28</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G22" s="8" t="str">
-        <f>B28</f>
+        <f t="shared" si="2"/>
         <v>Trajectory Test Controls</v>
       </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="32"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="41"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="37"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
@@ -2118,17 +2118,17 @@
         <v>58</v>
       </c>
       <c r="F23" s="12">
-        <f>A29</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23" s="8" t="str">
-        <f>B29</f>
+        <f t="shared" si="2"/>
         <v>Obstacle Avoidance Controls</v>
       </c>
-      <c r="I23" s="30"/>
-      <c r="J23" s="32"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="41"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="37"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
@@ -2151,10 +2151,10 @@
         <f>B19</f>
         <v>Autonomous Takeoff &amp; Landing</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="33"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="41"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="38"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
@@ -2169,8 +2169,8 @@
       <c r="D25" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="39"/>
-      <c r="M25" s="41"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
@@ -2193,16 +2193,16 @@
         <f>B15</f>
         <v>Durataion</v>
       </c>
-      <c r="I26" s="20">
+      <c r="I26" s="25">
         <f>AVERAGE(AVERAGE(F26:F27),A8,AVERAGE(F26:F27),AVERAGE(F26:F27))</f>
         <v>0</v>
       </c>
-      <c r="J26" s="34" t="str">
+      <c r="J26" s="39" t="str">
         <f>B8</f>
         <v>Hardware Subsystem</v>
       </c>
-      <c r="L26" s="39"/>
-      <c r="M26" s="41"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
@@ -2222,13 +2222,13 @@
         <f>B20</f>
         <v>Payload</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="35"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="42"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="40"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="23"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="19">
         <v>0</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -2237,7 +2237,7 @@
       <c r="L28" s="18"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
+      <c r="A29" s="19">
         <v>0</v>
       </c>
       <c r="B29" s="14" t="s">

</xml_diff>

<commit_message>
Updating Testing with Target ID
</commit_message>
<xml_diff>
--- a/Technical/Testing/TestPlan.xlsx
+++ b/Technical/Testing/TestPlan.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FlyNet\Technical\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylordean/Documents/FlyNet/Technical/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="13965"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -667,16 +667,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,6 +737,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,7 +810,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1500,41 +1500,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:J24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H1" s="24" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H1" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="K1" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="K1" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="24"/>
+      <c r="L1" s="25"/>
       <c r="N1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>0</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="20">
         <v>42401</v>
       </c>
       <c r="G3" s="12">
@@ -1595,24 +1595,24 @@
         <f>B9</f>
         <v>Initial Camera Test</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="27">
         <f>AVERAGE(AVERAGE(G3:G7),A5,AVERAGE(G3:G7),AVERAGE(G3:G7))</f>
         <v>0</v>
       </c>
-      <c r="K3" s="41" t="str">
+      <c r="K3" s="42" t="str">
         <f>B5</f>
         <v>Guidance Subsystem</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="21">
         <f>AVERAGE(AVERAGE(J3,J9,J15,J21,J26),A3,AVERAGE(J3,J9,J15,J21,J26),AVERAGE(J3,J9,J15,J21,J26))</f>
         <v>8.4375000000000006E-2</v>
       </c>
-      <c r="N3" s="21" t="str">
+      <c r="N3" s="22" t="str">
         <f>B3</f>
         <v>End of Semester Test Demo</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>0</v>
       </c>
@@ -1625,7 +1625,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="20">
         <v>42422</v>
       </c>
       <c r="G4" s="12">
@@ -1636,12 +1636,12 @@
         <f>B10</f>
         <v>Target Imaging</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="42"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="22"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="27"/>
+      <c r="K4" s="43"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>0</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="20">
         <v>42429</v>
       </c>
       <c r="G5" s="12">
@@ -1666,12 +1666,12 @@
         <v>Obstacle Perceived</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="42"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="27"/>
+      <c r="K5" s="43"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>0</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="20">
         <v>42415</v>
       </c>
       <c r="G6" s="12">
@@ -1696,12 +1696,12 @@
         <v>Obstacle Map</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="42"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="27"/>
+      <c r="K6" s="43"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>0</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="20">
         <v>42408</v>
       </c>
       <c r="G7" s="12">
@@ -1728,12 +1728,12 @@
       <c r="I7" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="43"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="27"/>
+      <c r="K7" s="44"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>0</v>
       </c>
@@ -1746,10 +1746,10 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="21"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>0</v>
       </c>
@@ -1762,8 +1762,11 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="44">
-        <v>42422</v>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
+        <v>42401</v>
       </c>
       <c r="G9" s="12">
         <f>A11</f>
@@ -1773,18 +1776,18 @@
         <f>B11</f>
         <v>Human Target ID</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="28">
         <f>AVERAGE(AVERAGE(G9:G13),A4,AVERAGE(G9:G13),AVERAGE(G9:G13))</f>
         <v>0</v>
       </c>
-      <c r="K9" s="28" t="str">
+      <c r="K9" s="29" t="str">
         <f>B4</f>
         <v>Tracking/ID Subsystem</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="22"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="21"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>0</v>
       </c>
@@ -1797,8 +1800,11 @@
       <c r="D10" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="44">
-        <v>42408</v>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="20">
+        <v>42415</v>
       </c>
       <c r="G10" s="12">
         <f t="shared" ref="G10:H12" si="0">A16</f>
@@ -1808,12 +1814,12 @@
         <f t="shared" si="0"/>
         <v>Target Estimation</v>
       </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="29"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="28"/>
+      <c r="K10" s="30"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>0</v>
       </c>
@@ -1826,8 +1832,11 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="44">
-        <v>42429</v>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="20">
+        <v>42408</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
@@ -1837,12 +1846,12 @@
         <f t="shared" si="0"/>
         <v>Multiple targets</v>
       </c>
-      <c r="J11" s="27"/>
-      <c r="K11" s="29"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="28"/>
+      <c r="K11" s="30"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>0</v>
       </c>
@@ -1855,8 +1864,11 @@
       <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="44">
-        <v>42415</v>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="20">
+        <v>42422</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
@@ -1866,12 +1878,12 @@
         <f t="shared" si="0"/>
         <v>Target Estimate Update</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="29"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="28"/>
+      <c r="K12" s="30"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>0</v>
       </c>
@@ -1884,8 +1896,11 @@
       <c r="D13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="44">
-        <v>42401</v>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="20">
+        <v>42429</v>
       </c>
       <c r="G13" s="12">
         <f>A25</f>
@@ -1895,12 +1910,12 @@
         <f>B25</f>
         <v>Target Accuracy and Range</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="30"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="22"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="28"/>
+      <c r="K13" s="31"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>0</v>
       </c>
@@ -1917,10 +1932,10 @@
         <v>69</v>
       </c>
       <c r="G14"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="21"/>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>0.75</v>
       </c>
@@ -1933,7 +1948,7 @@
       <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="20">
         <v>42415</v>
       </c>
       <c r="G15" s="12">
@@ -1944,18 +1959,18 @@
         <f t="shared" si="1"/>
         <v>Collision Correction Planning</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="35">
         <f>AVERAGE(AVERAGE(G15:G19),A6,AVERAGE(G15:G19),AVERAGE(G15:G19))</f>
         <v>0</v>
       </c>
-      <c r="K15" s="31" t="str">
+      <c r="K15" s="32" t="str">
         <f>B6</f>
         <v>Planning Subsystem</v>
       </c>
-      <c r="M15" s="20"/>
-      <c r="N15" s="22"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="21"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>0</v>
       </c>
@@ -1968,7 +1983,7 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="20">
         <v>42401</v>
       </c>
       <c r="G16" s="12">
@@ -1979,12 +1994,12 @@
         <f t="shared" si="1"/>
         <v>Trajectory Test Planning</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="32"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="22"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16" s="35"/>
+      <c r="K16" s="33"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>0</v>
       </c>
@@ -1997,7 +2012,7 @@
       <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="20">
         <v>42408</v>
       </c>
       <c r="G17" s="12">
@@ -2008,12 +2023,12 @@
         <f t="shared" si="1"/>
         <v>Obstacle Avoidance Planning</v>
       </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="32"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J17" s="35"/>
+      <c r="K17" s="33"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="23"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>0</v>
       </c>
@@ -2026,7 +2041,7 @@
       <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="20">
         <v>42422</v>
       </c>
       <c r="G18" s="12">
@@ -2036,12 +2051,12 @@
       <c r="H18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="32"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="22"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="35"/>
+      <c r="K18" s="33"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>0</v>
       </c>
@@ -2054,7 +2069,7 @@
       <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="20">
         <v>42429</v>
       </c>
       <c r="G19" s="12">
@@ -2064,12 +2079,12 @@
       <c r="H19" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="33"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="22"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="35"/>
+      <c r="K19" s="34"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>0.75</v>
       </c>
@@ -2082,10 +2097,10 @@
       <c r="D20" t="s">
         <v>46</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="22"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M20" s="21"/>
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>0</v>
       </c>
@@ -2098,7 +2113,7 @@
       <c r="D21" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="20">
         <v>42429</v>
       </c>
       <c r="G21" s="12">
@@ -2109,18 +2124,18 @@
         <f t="shared" si="2"/>
         <v>Collision Correction Controls</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="36">
         <f>AVERAGE(AVERAGE(G21:G24),A7,AVERAGE(G21:G24),AVERAGE(G21:G24))</f>
         <v>0</v>
       </c>
-      <c r="K21" s="36" t="str">
+      <c r="K21" s="37" t="str">
         <f>B7</f>
         <v>Controls Subsystem</v>
       </c>
-      <c r="M21" s="20"/>
-      <c r="N21" s="22"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="21"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>0</v>
       </c>
@@ -2133,7 +2148,7 @@
       <c r="D22" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="20">
         <v>42415</v>
       </c>
       <c r="G22" s="12">
@@ -2144,12 +2159,12 @@
         <f t="shared" si="2"/>
         <v>Trajectory Test Controls</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="37"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="22"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="36"/>
+      <c r="K22" s="38"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>0</v>
       </c>
@@ -2162,7 +2177,7 @@
       <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="20">
         <v>42422</v>
       </c>
       <c r="G23" s="12">
@@ -2173,12 +2188,12 @@
         <f t="shared" si="2"/>
         <v>Obstacle Avoidance Controls</v>
       </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="37"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="22"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="36"/>
+      <c r="K23" s="38"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>0</v>
       </c>
@@ -2191,7 +2206,7 @@
       <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="20">
         <v>42408</v>
       </c>
       <c r="G24" s="12">
@@ -2202,12 +2217,12 @@
         <f>B19</f>
         <v>Autonomous Takeoff &amp; Landing</v>
       </c>
-      <c r="J24" s="35"/>
-      <c r="K24" s="38"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="22"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="36"/>
+      <c r="K24" s="39"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>0</v>
       </c>
@@ -2220,10 +2235,10 @@
       <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="22"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M25" s="21"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>0</v>
       </c>
@@ -2239,7 +2254,7 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="20">
         <v>42401</v>
       </c>
       <c r="G26" s="12">
@@ -2250,18 +2265,18 @@
         <f>B15</f>
         <v>Durataion</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="26">
         <f>AVERAGE(AVERAGE(G26:G27),A8,AVERAGE(G26:G27),AVERAGE(G26:G27))</f>
         <v>0.5625</v>
       </c>
-      <c r="K26" s="39" t="str">
+      <c r="K26" s="40" t="str">
         <f>B8</f>
         <v>Hardware Subsystem</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="22"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="21"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>0</v>
       </c>
@@ -2271,7 +2286,7 @@
       <c r="E27">
         <v>2</v>
       </c>
-      <c r="F27" s="44">
+      <c r="F27" s="20">
         <v>42401</v>
       </c>
       <c r="G27" s="12">
@@ -2282,12 +2297,12 @@
         <f>B20</f>
         <v>Payload</v>
       </c>
-      <c r="J27" s="25"/>
-      <c r="K27" s="40"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="23"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="26"/>
+      <c r="K27" s="41"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>0</v>
       </c>
@@ -2296,7 +2311,7 @@
       </c>
       <c r="M28" s="18"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>0</v>
       </c>
@@ -2308,13 +2323,13 @@
       </c>
       <c r="M29" s="18"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M30" s="18"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M31" s="18"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K32" s="13"/>
       <c r="N32" s="13"/>
     </row>
@@ -2547,10 +2562,5 @@
     <hyperlink ref="B29" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating target tracking test progress
</commit_message>
<xml_diff>
--- a/Technical/Testing/TestPlan.xlsx
+++ b/Technical/Testing/TestPlan.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FlyNet\Technical\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylordean/Documents/FlyNet/Technical/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19380"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18940" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>Test</t>
   </si>
@@ -87,9 +87,6 @@
     <t>1.1.3</t>
   </si>
   <si>
-    <t>Human Target ID</t>
-  </si>
-  <si>
     <t>1.2.1</t>
   </si>
   <si>
@@ -114,30 +111,15 @@
     <t>Endurance test, while searching, full payload. Measure Distance traveled as well</t>
   </si>
   <si>
-    <t>Target Estimation</t>
-  </si>
-  <si>
     <t>2.1.1</t>
   </si>
   <si>
     <t>Estimate position to withing 0.5 meters</t>
   </si>
   <si>
-    <t>Multiple targets</t>
-  </si>
-  <si>
     <t>2.1.2</t>
   </si>
   <si>
-    <t>At least 2 targets estimated and ID</t>
-  </si>
-  <si>
-    <t>Target Estimate Update</t>
-  </si>
-  <si>
-    <t>Track targets, each updated position should be 10 Hz</t>
-  </si>
-  <si>
     <t>Autonomous Takeoff &amp; Landing</t>
   </si>
   <si>
@@ -181,12 +163,6 @@
   </si>
   <si>
     <t>Target Accuracy and Range</t>
-  </si>
-  <si>
-    <t>8.3.1, 8.3.2</t>
-  </si>
-  <si>
-    <t>Detect tags at 95% accuracy, find the maximum distance</t>
   </si>
   <si>
     <t>Component
@@ -214,9 +190,6 @@
     <t>End of Semester Test Demo</t>
   </si>
   <si>
-    <t xml:space="preserve">Correctly locate targets 95% of time </t>
-  </si>
-  <si>
     <t>Receive and Transmit Test</t>
   </si>
   <si>
@@ -261,9 +234,6 @@
 Completed by</t>
   </si>
   <si>
-    <t>1.1.4</t>
-  </si>
-  <si>
     <t>2.1.3, 2.2.1</t>
   </si>
   <si>
@@ -285,9 +255,6 @@
     <t>Record images, load into processing software on the quad</t>
   </si>
   <si>
-    <t>Calculate and demonstrate distance for at least 95% human ID</t>
-  </si>
-  <si>
     <t>SLAM accuracy and positioning at minimum speed</t>
   </si>
   <si>
@@ -304,6 +271,36 @@
   </si>
   <si>
     <t>7.2.1, 7.2.2</t>
+  </si>
+  <si>
+    <t>Target position update should occur at 10Hz</t>
+  </si>
+  <si>
+    <t>Correctly locate targets 95% of time with 0.5 m accuracy</t>
+  </si>
+  <si>
+    <t>Identify human target 95% of the time</t>
+  </si>
+  <si>
+    <t>Multiple targets tracked simultaneously</t>
+  </si>
+  <si>
+    <t>Target Estimation Accuracy</t>
+  </si>
+  <si>
+    <t>Multiple Targets Tracking</t>
+  </si>
+  <si>
+    <t>Target Estimate Update Frequency</t>
+  </si>
+  <si>
+    <t>Detect targets with 0.5m accuracy, find the maximum distance</t>
+  </si>
+  <si>
+    <t>Human Target Probability of Detection</t>
+  </si>
+  <si>
+    <t>1.1.3, 1.1.4, 8.3.1, 8.3.2</t>
   </si>
 </sst>
 </file>
@@ -1507,42 +1504,42 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H1" s="25" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I1" s="25"/>
       <c r="K1" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L1" s="25"/>
       <c r="N1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1551,38 +1548,38 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="M2" s="11"/>
       <c r="N2" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>0</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1614,14 +1611,14 @@
       </c>
       <c r="M3" s="21">
         <f>AVERAGE(AVERAGE(J3,J9,J15,J21,J26),A3,AVERAGE(J3,J9,J15,J21,J26),AVERAGE(J3,J9,J15,J21,J26))</f>
-        <v>9.5625000000000002E-2</v>
+        <v>0.12374999999999999</v>
       </c>
       <c r="N3" s="22" t="str">
         <f>B3</f>
         <v>End of Semester Test Demo</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>0</v>
       </c>
@@ -1629,7 +1626,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1653,7 +1650,7 @@
       <c r="M4" s="21"/>
       <c r="N4" s="23"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>0</v>
       </c>
@@ -1661,7 +1658,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1686,7 +1683,7 @@
       <c r="M5" s="21"/>
       <c r="N5" s="23"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>0</v>
       </c>
@@ -1719,7 +1716,7 @@
       <c r="M6" s="21"/>
       <c r="N6" s="23"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>0</v>
       </c>
@@ -1727,7 +1724,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -1747,14 +1744,14 @@
         <v>Visual Odometry Verification and Characterization</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="44"/>
       <c r="M7" s="21"/>
       <c r="N7" s="23"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>0</v>
       </c>
@@ -1770,7 +1767,7 @@
       <c r="M8" s="21"/>
       <c r="N8" s="23"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>0</v>
       </c>
@@ -1778,10 +1775,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1791,15 +1788,15 @@
       </c>
       <c r="G9" s="12">
         <f>A11</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="6" t="str">
         <f>B11</f>
-        <v>Human Target ID</v>
+        <v>Human Target Probability of Detection</v>
       </c>
       <c r="J9" s="28">
         <f>AVERAGE(AVERAGE(G9:G13),A4,AVERAGE(G9:G13),AVERAGE(G9:G13))</f>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="K9" s="29" t="str">
         <f>B4</f>
@@ -1808,7 +1805,7 @@
       <c r="M9" s="21"/>
       <c r="N9" s="23"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>0</v>
       </c>
@@ -1819,7 +1816,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1833,57 +1830,57 @@
       </c>
       <c r="H10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Target Estimation</v>
+        <v>Target Estimation Accuracy</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="30"/>
       <c r="M10" s="21"/>
       <c r="N10" s="23"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="20">
         <v>42408</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Multiple targets</v>
+        <v>Multiple Targets Tracking</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="30"/>
       <c r="M11" s="21"/>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>0</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1897,25 +1894,25 @@
       </c>
       <c r="H12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Target Estimate Update</v>
+        <v>Target Estimate Update Frequency</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="30"/>
       <c r="M12" s="21"/>
       <c r="N12" s="23"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>0</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1936,41 +1933,41 @@
       <c r="M13" s="21"/>
       <c r="N13" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>0</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G14"/>
       <c r="M14" s="21"/>
       <c r="N14" s="23"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>0.85</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1997,18 +1994,18 @@
       <c r="M15" s="21"/>
       <c r="N15" s="23"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>0</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -2029,18 +2026,18 @@
       <c r="M16" s="21"/>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2061,18 +2058,18 @@
       <c r="M17" s="21"/>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>0</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -2085,25 +2082,25 @@
         <v>0</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="33"/>
       <c r="M18" s="21"/>
       <c r="N18" s="23"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>0</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2116,41 +2113,41 @@
         <v>0</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J19" s="35"/>
       <c r="K19" s="34"/>
       <c r="M19" s="21"/>
       <c r="N19" s="23"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>0.85</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="M20" s="21"/>
       <c r="N20" s="23"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>0</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -2177,18 +2174,18 @@
       <c r="M21" s="21"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>0</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2209,18 +2206,18 @@
       <c r="M22" s="21"/>
       <c r="N22" s="23"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>0</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2241,18 +2238,18 @@
       <c r="M23" s="21"/>
       <c r="N23" s="23"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>0</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -2273,34 +2270,34 @@
       <c r="M24" s="21"/>
       <c r="N24" s="23"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>0</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="M25" s="21"/>
       <c r="N25" s="23"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>0</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2327,18 +2324,18 @@
       <c r="M26" s="21"/>
       <c r="N26" s="23"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>0</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
         <v>20</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -2359,46 +2356,46 @@
       <c r="M27" s="21"/>
       <c r="N27" s="24"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>0</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="M28" s="18"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>0</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
         <v>23</v>
       </c>
-      <c r="D29" t="s">
-        <v>24</v>
-      </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="M29" s="18"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M30" s="18"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M31" s="18"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K32" s="13"/>
       <c r="N32" s="13"/>
     </row>
@@ -2610,14 +2607,14 @@
     <hyperlink ref="B8" r:id="rId6"/>
     <hyperlink ref="B9" r:id="rId7"/>
     <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId9" display="Human Target ID"/>
     <hyperlink ref="B12" r:id="rId10"/>
     <hyperlink ref="B13" r:id="rId11"/>
     <hyperlink ref="B14" r:id="rId12"/>
     <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B16" r:id="rId14" display="Target Estimation"/>
+    <hyperlink ref="B17" r:id="rId15" display="Multiple targets"/>
+    <hyperlink ref="B18" r:id="rId16" display="Target Estimate Update"/>
     <hyperlink ref="B19" r:id="rId17"/>
     <hyperlink ref="B20" r:id="rId18"/>
     <hyperlink ref="B21" r:id="rId19"/>

</xml_diff>

<commit_message>
Final Test Plan Update
</commit_message>
<xml_diff>
--- a/Technical/Testing/TestPlan.xlsx
+++ b/Technical/Testing/TestPlan.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Drew/Desktop/FlyNet/Technical/Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FlyNet\Technical\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="860" windowWidth="25840" windowHeight="17460"/>
+    <workbookView xWindow="285" yWindow="855" windowWidth="25845" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -220,12 +220,6 @@
     <t>Now - February 29</t>
   </si>
   <si>
-    <t>April 18 - End Of Semester</t>
-  </si>
-  <si>
-    <t>March 1 - April 17</t>
-  </si>
-  <si>
     <t>Min People 
 Required</t>
   </si>
@@ -301,6 +295,12 @@
   </si>
   <si>
     <t>Correctly locate targets in the map 95% of time with 0.5 m accuracy</t>
+  </si>
+  <si>
+    <t>March 1 - End of Semester</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -1486,41 +1486,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H1" s="23" t="s">
         <v>62</v>
       </c>
       <c r="I1" s="23"/>
       <c r="K1" s="23" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="L1" s="23"/>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1531,13 +1528,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>45</v>
@@ -1557,7 +1554,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -1585,22 +1582,21 @@
       </c>
       <c r="J3" s="25">
         <f>AVERAGE(AVERAGE(G3:G7),A5,AVERAGE(G3:G7),AVERAGE(G3:G7))</f>
-        <v>0.28750000000000003</v>
+        <v>0.51249999999999996</v>
       </c>
       <c r="K3" s="40" t="str">
         <f>B5</f>
         <v>Guidance Subsystem</v>
       </c>
       <c r="M3" s="19">
-        <f>AVERAGE(AVERAGE(J3,J9,J15,J21,J26),A3,AVERAGE(J3,J9,J15,J21,J26),AVERAGE(J3,J9,J15,J21,J26))</f>
-        <v>0.4069687500000001</v>
-      </c>
-      <c r="N3" s="20" t="str">
-        <f>B3</f>
-        <v>End of Semester Test Demo</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f>AVERAGE(AVERAGE(J3,J9,J15,J21,J26),AVERAGE(J3,J9,J15,J21,J26),AVERAGE(J3,J9,J15,J21,J26))</f>
+        <v>0.72450000000000025</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>0.25</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1620,7 +1616,7 @@
         <v>42422</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="13" t="str">
         <f>B10</f>
@@ -1631,7 +1627,7 @@
       <c r="M4" s="19"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>0.25</v>
       </c>
@@ -1639,7 +1635,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1651,7 +1647,7 @@
         <v>42415</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="13" t="str">
         <f>B22</f>
@@ -1663,7 +1659,7 @@
       <c r="M5" s="19"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>0.5</v>
       </c>
@@ -1683,7 +1679,7 @@
         <v>42429</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="13" t="str">
         <f>B23</f>
@@ -1695,7 +1691,7 @@
       <c r="M6" s="19"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>0.5</v>
       </c>
@@ -1729,7 +1725,7 @@
       <c r="M7" s="19"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>0.75</v>
       </c>
@@ -1745,7 +1741,7 @@
       <c r="M8" s="19"/>
       <c r="N8" s="21"/>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f>G3</f>
         <v>0.75</v>
@@ -1754,10 +1750,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1786,10 +1782,10 @@
       <c r="M9" s="19"/>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f>G4</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1798,7 +1794,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1818,19 +1814,19 @@
       <c r="M10" s="19"/>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f>G9</f>
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1850,10 +1846,10 @@
       <c r="M11" s="19"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f>G15</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -1885,16 +1881,16 @@
       <c r="M12" s="19"/>
       <c r="N12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f>G16</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1917,7 +1913,7 @@
       <c r="M13" s="19"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>0.75</v>
       </c>
@@ -1940,7 +1936,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f>G26</f>
         <v>0.85</v>
@@ -1961,7 +1957,7 @@
         <v>42415</v>
       </c>
       <c r="G15" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H15" s="15" t="str">
         <f t="shared" ref="H15:H17" si="1">B12</f>
@@ -1969,7 +1965,7 @@
       </c>
       <c r="J15" s="33">
         <f>AVERAGE(AVERAGE(G15:G19),A6,AVERAGE(G15:G19),AVERAGE(G15:G19))</f>
-        <v>0.16250000000000003</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="K15" s="30" t="str">
         <f>B6</f>
@@ -1978,13 +1974,13 @@
       <c r="M15" s="19"/>
       <c r="N15" s="21"/>
     </row>
-    <row r="16" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f>G10</f>
         <v>0.9</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1999,7 +1995,7 @@
         <v>42401</v>
       </c>
       <c r="G16" s="6">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H16" s="15" t="str">
         <f t="shared" si="1"/>
@@ -2010,19 +2006,19 @@
       <c r="M16" s="19"/>
       <c r="N16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f>G11</f>
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2031,7 +2027,7 @@
         <v>42408</v>
       </c>
       <c r="G17" s="6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H17" s="15" t="str">
         <f t="shared" si="1"/>
@@ -2042,19 +2038,19 @@
       <c r="M17" s="19"/>
       <c r="N17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f>G12</f>
         <v>0.75</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -2063,7 +2059,7 @@
         <v>42422</v>
       </c>
       <c r="G18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="15" t="s">
         <v>53</v>
@@ -2073,7 +2069,7 @@
       <c r="M18" s="19"/>
       <c r="N18" s="21"/>
     </row>
-    <row r="19" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f>G24</f>
         <v>1</v>
@@ -2082,7 +2078,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -2094,7 +2090,7 @@
         <v>42429</v>
       </c>
       <c r="G19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>41</v>
@@ -2104,7 +2100,7 @@
       <c r="M19" s="19"/>
       <c r="N19" s="21"/>
     </row>
-    <row r="20" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f>G27</f>
         <v>0.85</v>
@@ -2113,7 +2109,7 @@
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -2121,10 +2117,10 @@
       <c r="M20" s="19"/>
       <c r="N20" s="21"/>
     </row>
-    <row r="21" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f>G18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
@@ -2142,7 +2138,7 @@
         <v>42429</v>
       </c>
       <c r="G21" s="6">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H21" s="17" t="str">
         <f t="shared" ref="H21:H23" si="2">B27</f>
@@ -2150,7 +2146,7 @@
       </c>
       <c r="J21" s="34">
         <f>AVERAGE(AVERAGE(G21:G24),A7,AVERAGE(G21:G24),AVERAGE(G21:G24))</f>
-        <v>0.71562500000000007</v>
+        <v>0.76250000000000007</v>
       </c>
       <c r="K21" s="35" t="str">
         <f>B7</f>
@@ -2159,16 +2155,16 @@
       <c r="M21" s="19"/>
       <c r="N21" s="21"/>
     </row>
-    <row r="22" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f>G5</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -2191,10 +2187,10 @@
       <c r="M22" s="19"/>
       <c r="N22" s="21"/>
     </row>
-    <row r="23" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f>G6</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
@@ -2223,10 +2219,10 @@
       <c r="M23" s="19"/>
       <c r="N23" s="21"/>
     </row>
-    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f>G19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
@@ -2255,7 +2251,7 @@
       <c r="M24" s="19"/>
       <c r="N24" s="21"/>
     </row>
-    <row r="25" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f>G13</f>
         <v>0.75</v>
@@ -2264,10 +2260,10 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
         <v>50</v>
@@ -2275,7 +2271,7 @@
       <c r="M25" s="19"/>
       <c r="N25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f>G7</f>
         <v>0.75</v>
@@ -2287,7 +2283,7 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2313,7 +2309,7 @@
       <c r="M26" s="19"/>
       <c r="N26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>0.5</v>
       </c>
@@ -2344,7 +2340,7 @@
       <c r="M27" s="19"/>
       <c r="N27" s="22"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <f>G22</f>
         <v>0.9</v>
@@ -2353,14 +2349,14 @@
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <f>G23</f>
         <v>0.75</v>
@@ -2379,13 +2375,13 @@
       </c>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K32" s="7"/>
       <c r="N32" s="7"/>
     </row>

</xml_diff>